<commit_message>
Added my Sub Group
</commit_message>
<xml_diff>
--- a/CubeSatTeamRoster.xlsx
+++ b/CubeSatTeamRoster.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Desktop\CubeSat\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Charles Denis</t>
   </si>
@@ -123,6 +118,9 @@
   </si>
   <si>
     <t>Communications</t>
+  </si>
+  <si>
+    <t>ADNCS</t>
   </si>
 </sst>
 </file>
@@ -494,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,7 +503,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +556,9 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>